<commit_message>
removed empty file, added reference
Former-commit-id: d11dc12d12c7f77e76ba10f120dca104baa09505
Former-commit-id: 21622e2fe245a5d9daecb043b58546678e54b2a1
</commit_message>
<xml_diff>
--- a/data/japan_costs/advanced fossil-ccs-nuc.xlsx
+++ b/data/japan_costs/advanced fossil-ccs-nuc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alley cat\Documents\GitHub\i2cner\data\japan_costs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arfc\Documents\GitHub\i2cner\data\japan_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702E3F69-E0F0-41C3-AAC9-07281CE4377B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1F2D5B-2428-4F1C-AC24-658791D5F0A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="2610" windowWidth="21600" windowHeight="11325" xr2:uid="{558254C2-F576-4D72-B799-A1AA36A7D720}"/>
+    <workbookView xWindow="1680" yWindow="2970" windowWidth="19755" windowHeight="10155" xr2:uid="{558254C2-F576-4D72-B799-A1AA36A7D720}"/>
   </bookViews>
   <sheets>
     <sheet name="Coal" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>https://atb.nrel.gov/electricity/2017/index.html?t=cc&amp;s=cx</t>
   </si>
@@ -95,13 +95,16 @@
   </si>
   <si>
     <t>Not important</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/outlooks/capitalcost/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +117,14 @@
       <color rgb="FF333333"/>
       <name val="Georgia"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,15 +144,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,7 +471,7 @@
   <dimension ref="A2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +509,7 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -523,7 +537,7 @@
       <c r="E5">
         <v>83.75</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -540,6 +554,9 @@
       <c r="E7">
         <v>11.33</v>
       </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -572,8 +589,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{CA70AB4F-732A-4A66-AB18-370BFC5B3DA3}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{9B0787CA-7F70-4F7E-9C06-6A5372AB84B0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>